<commit_message>
comited in 2nd dec
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -50,7 +50,7 @@
     <t>kietmca14@gmail.com</t>
   </si>
   <si>
-    <t>123456ABC</t>
+    <t>abcdefgh</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,7 +384,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>